<commit_message>
Alle profilene er med (unntatt procedure)
</commit_message>
<xml_diff>
--- a/StructureDefinition-no-basis-Address.xlsx
+++ b/StructureDefinition-no-basis-Address.xlsx
@@ -24,7 +24,7 @@
     <t>URL</t>
   </si>
   <si>
-    <t>http://hl7.no/fhir/no-basis/StructureDefinition/no-basis-Address</t>
+    <t>http://hl7.no/fhir/StructureDefinition/no-basis-Address</t>
   </si>
   <si>
     <t>Version</t>
@@ -335,7 +335,7 @@
 user content</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {http://hl7.no/fhir/no-basis/StructureDefinition/no-basis-address-official}
+    <t xml:space="preserve">Extension {http://hl7.no/fhir/StructureDefinition/no-basis-address-official}
 </t>
   </si>
   <si>
@@ -352,7 +352,7 @@
 urban district</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {http://hl7.no/fhir/no-basis/StructureDefinition/no-basis-urban-district}
+    <t xml:space="preserve">Extension {http://hl7.no/fhir/StructureDefinition/no-basis-urban-district}
 </t>
   </si>
   <si>
@@ -365,7 +365,7 @@
     <t>propertyInformation</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {http://hl7.no/fhir/no-basis/StructureDefinition/no-basis-propertyinformation}
+    <t xml:space="preserve">Extension {http://hl7.no/fhir/StructureDefinition/no-basis-propertyinformation}
 </t>
   </si>
   <si>
@@ -574,7 +574,7 @@
     <t>municipalitycode</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {http://hl7.no/fhir/no-basis/StructureDefinition/no-basis-municipalitycode}
+    <t xml:space="preserve">Extension {http://hl7.no/fhir/StructureDefinition/no-basis-municipalitycode}
 </t>
   </si>
   <si>

</xml_diff>